<commit_message>
Made changes to sort by congressional district and last name
</commit_message>
<xml_diff>
--- a/src/WSGC_Recipient_Data_Report.xlsx
+++ b/src/WSGC_Recipient_Data_Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19360" windowHeight="16060" tabRatio="1000" activeTab="11"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="33440" windowHeight="16060" tabRatio="1000" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="AOP" sheetId="2" r:id="rId1"/>
@@ -14,11 +14,14 @@
     <sheet name="HEI" sheetId="6" r:id="rId5"/>
     <sheet name="IIP" sheetId="7" r:id="rId6"/>
     <sheet name="NIP" sheetId="8" r:id="rId7"/>
-    <sheet name="RIP" sheetId="9" r:id="rId8"/>
-    <sheet name="SBS" sheetId="10" r:id="rId9"/>
-    <sheet name="SIP" sheetId="11" r:id="rId10"/>
-    <sheet name="SSI" sheetId="12" r:id="rId11"/>
-    <sheet name="UGR" sheetId="13" r:id="rId12"/>
+    <sheet name="OPP" sheetId="15" r:id="rId8"/>
+    <sheet name="RIP" sheetId="9" r:id="rId9"/>
+    <sheet name="SBS" sheetId="10" r:id="rId10"/>
+    <sheet name="SIP" sheetId="11" r:id="rId11"/>
+    <sheet name="SSI" sheetId="12" r:id="rId12"/>
+    <sheet name="UGR" sheetId="13" r:id="rId13"/>
+    <sheet name="UGS" sheetId="14" r:id="rId14"/>
+    <sheet name="USIP" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="447">
   <si>
     <t>Name</t>
   </si>
@@ -1589,6 +1592,337 @@
   <si>
     <t>none</t>
   </si>
+  <si>
+    <t>Undergraduate Student Scholarship; $2000.00</t>
+  </si>
+  <si>
+    <t>Tyler Rasmussen is a sophomore at University of Wisconsin-Fox Valley majoring in Mechanical Engineering. He presently holds a position in parcel recovery for various airlines at the Austin Straubel and Appleton International Airports. Tyler has been elected president of the 2016-17 Chemistry Club on campus and is also a member of the Engineering Club. In his free time, he utilizes his mechanical aptitude by customizing his car. After attaining his bachelor’s degree, he plans to further his education in
+areas such as astrophysics, chemistry, and nanotechnology. Tyler plans to utilize his education by working in the aerospace industry.</t>
+  </si>
+  <si>
+    <t>Ryan Kisiolek</t>
+  </si>
+  <si>
+    <t>Sophomore, Microbiology</t>
+  </si>
+  <si>
+    <t>I am a nontraditional student, I return to school to school after working in staging and
+construction for 15 years. I am a first generation college student and my major is microbiology with a minor in chemistry. I have sat as a officer on the student government every year I have been at school and I am also the president of the astronomy club this year. I am the team leader for our RockSat-C team and I am looking forward to continuing to work with biology and space related studies.</t>
+  </si>
+  <si>
+    <t>Rickie Dodge</t>
+  </si>
+  <si>
+    <t>My name is Rickie Lee Dodge, I am currently a sophomore at the College of Menominee
+Nation. I am studying Pre-environmental engineering technology and business administration, I hope to graduate in the Spring of 2017 with both degrees. After I finish at CMN I would like to attend UW system to work towards my bachelor’s degree in engineering. I am an active student in the school and the community. I am president of the AISES club and would also am in charge of the rockets for FNL. I am currently actively involved in one fellowship, Women in stem series seminars. I also do other research and online classes for renewable energy. I attend school full time where I also work part time as a tutor and get involved in many activities around campus and programs with Lisa Bosman. In my free time I like to spend time relaxing and helping others push past their struggles.</t>
+  </si>
+  <si>
+    <t>Reid Ribble</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celestine Ananda </t>
+  </si>
+  <si>
+    <t>Celestine Ananda is a freshman Physics &amp; Mathematics major at Carthage College. Her interest in physics began with a fundamental and fruitful curiosity in the mathematics and laws that govern our universe. She keeps herself busy participating in the Canopy Near-Infrared Observing Project (CaNOP) where she serves as the team co-lead of the CubeSat Attitude Determination and Control System. She plans to spend the summer designing and building a testing facility (Helmholtz cage) for the subsystem’s components and analyzing simulations at Carthage College. Celestine will continue to keep herself busy as the 2017-2018 Society of Physics Students President. She has developed interests in several career paths in the space sciences industry and has a strong passion for learning.</t>
+  </si>
+  <si>
+    <t>Karstan Hintz</t>
+  </si>
+  <si>
+    <t>Karsten Hintz is a senior at the University of Wisconsin Stevens Point and is double majoring in physics and math, and has a minor in anthropology. He works as a trigonometry, calculus and chemistry tutor in the Tutor-Learning Center at UW-Stevens Point. Karsten also spends his time lecturing to kids and adults as a planetarium lecturer at the Allen F. Blocher Planetarium, and as an observatory operator at
+the Arthur J. Pejsa Observatory. Karsten recalls being interested in science as a child and developed a particular curiosity in the science of physics and astronomy after he was gifted a telescope at a young age. He plans to continue nurturing his interest in physics and astronomy at the undergraduate level and eventually going on to pursue a doctorate in physics or math. After completing his doctorate Karsten hopes to pursue a career in academic research.</t>
+  </si>
+  <si>
+    <t>Sophomore, Electrical Engineering</t>
+  </si>
+  <si>
+    <t>My name is Nicole Jackson. I am a freshman at the Milwaukee School of Engineering. This is my first time working with rocketry, however I have built a Van’s RV-12 Airplane. I recently obtained my Private Pilot’s License in RV-12. I am very passionate about aviation and aircraft. I am helping to work on the completion of a second RV-12 that is being created at my local high school. I attend multiple Fly-ins throughout the year and enjoy learning more about General Aviation.</t>
+  </si>
+  <si>
+    <t>Raised at Florence, South Carolina, Xavier James currently attends University of Wisconsin- La Crosse pursuing a degree in physics and mathematics. After graduating, he plans to continue his education and obtain his Ph.D. in nuclear physics. Once complete, Xavier will then pursue a career in the research field of nuclear science.</t>
+  </si>
+  <si>
+    <t>Madeline Kothe</t>
+  </si>
+  <si>
+    <t>Maddie is a fourth year student at the University of Wisconsin-Madison with one year of school remaining. She is studying engineering mechanics with an option in astronautics to allow her to explore her interest in space. One of her favorite classes is satellite dynamics and she is looking forward to the challenges and triumphs that accompany the two semesters of senior design coming next year. Beyond the classroom, she is involved in many unique activities. These include working at Sierra Nevada and keeping up with NASA and astronauts on a daily basis through social media. The activity she is most passionate about is waterskiing for the Mad-City Ski Team. This allows her to not only improve on her own skills, such as swivel skiing, but also to take on a leadership role as the captain of the ballet line. Maddie is excited for the opportunity to have been awarded this scholarship and plans to put it towards her tuition- specifically she will be taking a class at UW-Madison to receive her pilot’s license.</t>
+  </si>
+  <si>
+    <t>Alecio Madrid is currently a junior at the University of Wisconsin-Madison
+studying Applied Mathematics, Astronomy, Chemistry, Computer Science, and
+Physics. He is originally from Denver, Colorado, but his parents currently living in
+Reading, United Kingdom. He is currently researching magnetic fields within star
+forming molecular gas in the milky way galaxy, and is looking forward to
+continuing his research over the next year. His hobbies include traveling, reading,
+and coding, and he has a passion for space and science. He is grateful for this
+opportunity, and looking forward to the upcoming months.</t>
+  </si>
+  <si>
+    <t>Jared Maraccini</t>
+  </si>
+  <si>
+    <t>Senior Physics</t>
+  </si>
+  <si>
+    <t>My name is Jared Maraccini and I am from Kenosha, WI. I am now a junior at the
+Milwaukee School of Engineering studying mechanical engineering and physics. My whole life I’ve been a student-athlete and continue to do so as I run cross country and track here year-round, as well as represent the men’s track team at our school’s Student-Athlete Advisory Committee. During my freshman year at MSOE I heard about the AIAA club on campus and attended as many meetings as I could. Through those meetings I learned about the collegiate rocket competition and got involved my sophomore year. I also heard about a summer internship that was also through the WSGC and was awarded it for the summer after my freshman year. Working with the AIAA chapter on campus and the WSGC have been major highlights during my time at MSOE and I hope to stay involved with both for the rest of my time here.</t>
+  </si>
+  <si>
+    <t>Evan Matel</t>
+  </si>
+  <si>
+    <t>Freshman, Astrophysics</t>
+  </si>
+  <si>
+    <t>Evan Matel is an incoming freshman at UW-Parkside, and is ecstatic to fulfill his
+curiosity for ‘how the universe works’ by pursuing a major in Physics. The stars and ‘life beyond our planet’ are very compelling subjects to Evan, and he plans on attending UW-
+Milwaukee his sophomore year onward in order to add an Astronomy emphasis to his degree. After obtaining his undergraduate degree, Evan plans on attending UW-Madison
+to earn a doctorate degree in Astrophysics.</t>
+  </si>
+  <si>
+    <t>Lisa Mowery</t>
+  </si>
+  <si>
+    <t>Junior, Geophysics</t>
+  </si>
+  <si>
+    <t>Lisa Mowery is a student at the University of Wisconsin-Milwaukee. She is pursuing a
+B.S. in Geophysics and is in her junior year. She is a first-generation college student and the first woman in her family to attend a four-year university. Miss Mowery has attained Sophomore Honors, has been on the Dean’s List for the last two years, and has won the Access to Excellence Scholarship in 2016. She has previously performed field work in Nevada regarding ancient coral reef systems and their resilience to local extinction events. She is currently performing undergraduate research studying hydrothermal effects on volcanic rocks in Iceland. In addition to her studies, Miss Mowery is an active volunteer with several local organizations. She works with Milwaukee Riverkeeper, monitoring various stream sites within the Milwaukee River Basin and with the Wisconsin Bat Program monitoring bat colony populations in response to the recent outbreak of white-nose syndrome. She currently resides in Milwaukee, WI and can be contacted at LMowery@uwm.edu.</t>
+  </si>
+  <si>
+    <t>Grant Petik</t>
+  </si>
+  <si>
+    <t>Freshman, Mechanical Engieering</t>
+  </si>
+  <si>
+    <t>Grant Petik, 18, is currently a senior at Fond du Lac High School, where he has been
+studying Math, Science, and Engineering since his freshman year. Throughout high school, he has taken rigorous courses at the college level including Advanced Physics, Chemistry,
+Calculus I &amp; II, Engineering Mechanics: Statics, and The History of Rock and Roll. Next fall,
+Grant will be attending the University of Wisconsin at Madison to pursue an undergraduate degree in Engineering Mechanics. While he plans to continue onto the graduate level, Grant aspires to work as an engineer for NASA, Lockheed Martin, SpaceX, or a similar organization to push the boundaries of our technology and to better understand our place in the universe. Outside of the classroom, Grant can be found enjoying his musical pursuits: Playing the trombone in jazz band, starring in his school musicals, or just playing his guitar. Finally, Grant would like to thank the WSGC for their generous support of his educational endeavors, as well as recognize the indispensable congressional support of science and education that can offers scholarships such as this.</t>
+  </si>
+  <si>
+    <t>Olivia Rasmussen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mark Pocan</t>
+  </si>
+  <si>
+    <t>Kaisa Crawford-Taylor</t>
+  </si>
+  <si>
+    <t>Ever since she was 8 years old, Kaisa has wanted to become a theoretical astrophysicist. At 18 years old she is accomplishing her dream. Throughout high school she has done independent research for the Junior Science and Humanities Symposium to computationally analyze Quasars and Super Massive Black Hole Binary candidates. As a freshman at the University of Wisconsin La Crosse she is working with Dr. Sallmen on calculating the various accelerations acting on a mirror fleet to find extra terrestrial life. She is also working with the company Fastenal to optimize their existing inventory distribution with machine learning. Her research has taken her to multiple national
+conferences and even to present at the 2016 White House Science Fair. Outside of astrophysics she also has a passion for art and plans to study abroad in Germany next spring.</t>
+  </si>
+  <si>
+    <t>Mark Vandenberg</t>
+  </si>
+  <si>
+    <t>Mark J Vandenberg is a freshman mechanical engineering student at the University of Wisconsin-Madison. In high school, his primary research focus was fluid dynamic interactions with air foil design using both experimental and computational methods. Currently, he is a cadet at Air Force ROTC Detachment 925, working towards his commission as a 2nd lieutenant in the United State Air Force, intending to serve in a technically intensive leadership role on aerospace related military acquisition projects.</t>
+  </si>
+  <si>
+    <t>Assistant Professor, Physics</t>
+  </si>
+  <si>
+    <t>Rock-Sat C</t>
+  </si>
+  <si>
+    <t>Brant Carlson is faculty advisor to Carthage College’s RockSat-X team. On the Carthage faculty since 2012, his research specialty is atmospheric electricity, specifically thunderstorms, lightning, and intense events called terrestrial gamma-ray flashes wherein a thunderstorm somehow emits higher energy radiation than any other natural process on Earth. Dr. Carlson’s research projects include simulation of the electrodynamics and plasma physics of the lightning channel, analysis of observations of lightning by satellites, analysis of energetic radiation produced by meter-long sparks in the lab, and instrument
+development, including construction of a network of electric field meters to deploy to local schools and participation in the development of the Atmosphere-Space Interactions Monitor, an instrument under construction to be launched to the international space station. Dr. Carlson holds a Ph.D. in physics from Stanford University and a bachelor of science degree in physics from the California Institute of Technology.</t>
+  </si>
+  <si>
+    <t>The project’s goal is to measure electromagnetic radiation produced by lightning in the atmosphere and lower ionosphere by mounting a student-designed and -built instrument on a sub-orbital rocket through participation in the RockSat-C program. The data collected will help better understand the process by which electromagnetic radiation from lightning is reflected and/or transmitted by the ionosphere. Such measurements have not previously been made in the lower ionosphere, so this project will shed light on the mechanism of energy reflection and escape as relevant to radiation belt dynamics in near-Earth space and
+electromagnetic interference at ground level. This project provides an excellent opportunity for students to gain experience with scientific and engineering best practices while working as a team participating in a high-profile program.</t>
+  </si>
+  <si>
+    <t>Sonny Nimityongskul</t>
+  </si>
+  <si>
+    <t>Faculty Associate, Engineering Physics</t>
+  </si>
+  <si>
+    <t>Robotic Mining</t>
+  </si>
+  <si>
+    <t>Sonny Nimityongskul is a lecturer in the Engineering Mechanics department at the University of Wisconsin-Madison. After receiving his Ph.D. from the UW-Madison, Sonny worked as a structural analyst for Cummins, where he specialized in predicting weld fatigue. After starting a family, Sonny returned to his alma mater to be a part-time lecturer and a full-time stay at home dad. In addition to teaching, he also advises the colligate rocket club and the lunar mining team.</t>
+  </si>
+  <si>
+    <t>Michael Swedish</t>
+  </si>
+  <si>
+    <t>Associate Professor, Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>NASA-sponsored Senior Design project</t>
+  </si>
+  <si>
+    <t>Michael Swedish is Associate Professor of Mechanical Engineering at the Milwaukee
+School of Engineering. He has been on the faculty for 31 years. His areas of expertise are
+Thermodynamics and Energy Systems, and resource utilization. He has prior years of industry experience, primarily in the electric power generation/utility sector. Professor Swedish has advised NASA Senior Design projects for the past ten years, working with technical advisers at the NASA centers, including Kennedy Space Center, Johnson Space Center, Marshall Space Flight Center, and Glenn Research Center.</t>
+  </si>
+  <si>
+    <t>CaNOP - CubeSat</t>
+  </si>
+  <si>
+    <t>Canopy Near-Infrared Observing Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Canopy Near-IR Observing Project will utilize a multispectral pushbroom imager in a 3U CubeSat to carry out spectrally resolved imaging of global forest regions with spectral resolution sufficient to reproduce early LandSat and MODIS missions. 
+Forests currently absorb as much as 30% of annual global anthropogenic carbon dioxide emissions (Schimel, 2014). Natural carbon flux is a critical yet poorly understood component of climate change, particularly in the mitigation of its effects. Many of the scientific questions around global forest carbon-uptake are large-scale questions of landscape ecology and therefore are appropriately addressed through space-based remote sensing. The Wisconsin Space Grant Consortium (WSGC) proposes to develop a CubeSat-based platform for performing multispectral imaging of forests around the world in an effort to support and understand large-scale biomass production and carbon sequestration in both mature and young second-growth forests. CaNOP will be a CubeSat platform for performing basic multispectral imaging of forest canopies in the Landsat Thematic Mapper bands TM2, TM3, and TM4, and in select MODIS bands.
+The specific scientific goals of this project are to image forests (which are categorized by biome), and collect reflectance data about the target regions. Illumination data (gathered in the visible and Near Infrared (NIR) spectra) will be used to compute the Normalized Difference Vegetation Index (NDVI), a ratio of the amount of light reflected in the NIR ranged compared to that of visible light. The comparison between young secondary and old-growth forests may help address a recent and paradoxical observation that suggests that primary forests are absorbing more carbon than their younger counterparts.
+The primary technological objective of the mission is to demonstrate that the types of landform observations made possible by LandSat and MODIS class instruments can be reproduced with comparable spectral resolutions using less expensive equipment and a CubeSat based platform.
+</t>
+  </si>
+  <si>
+    <t>Celestine Ananda</t>
+  </si>
+  <si>
+    <t>TeamMember7</t>
+  </si>
+  <si>
+    <t>TeamMember8</t>
+  </si>
+  <si>
+    <t>TeamMember9</t>
+  </si>
+  <si>
+    <t>TeamMember10</t>
+  </si>
+  <si>
+    <t>TeamMember11</t>
+  </si>
+  <si>
+    <t>TeamMember12</t>
+  </si>
+  <si>
+    <t>TeamMember13</t>
+  </si>
+  <si>
+    <t>TeamMember14</t>
+  </si>
+  <si>
+    <t>TeamMember15</t>
+  </si>
+  <si>
+    <t>TeamMember16</t>
+  </si>
+  <si>
+    <t>TeamMember17</t>
+  </si>
+  <si>
+    <t>TeamMember18</t>
+  </si>
+  <si>
+    <t>Joseph Wonsil</t>
+  </si>
+  <si>
+    <t>Nycole Wenner</t>
+  </si>
+  <si>
+    <t>Austin Weber</t>
+  </si>
+  <si>
+    <t>Jeremiah Munson</t>
+  </si>
+  <si>
+    <t>Caitlin Kitchen</t>
+  </si>
+  <si>
+    <t>Michael Huff</t>
+  </si>
+  <si>
+    <t>Michael Hernandez</t>
+  </si>
+  <si>
+    <t>Laura Hammock</t>
+  </si>
+  <si>
+    <t>Dan Gerloff</t>
+  </si>
+  <si>
+    <t>Charles Gallagher</t>
+  </si>
+  <si>
+    <t>Zachary Erickson</t>
+  </si>
+  <si>
+    <t>Kathleen Dziubinski</t>
+  </si>
+  <si>
+    <t>Michael Bisciglia</t>
+  </si>
+  <si>
+    <t>Max Becher</t>
+  </si>
+  <si>
+    <t>Nicholas Bartel</t>
+  </si>
+  <si>
+    <t>Jedidiah Barnes</t>
+  </si>
+  <si>
+    <t>Isaiah Jackson</t>
+  </si>
+  <si>
+    <t>Status7</t>
+  </si>
+  <si>
+    <t>Status8</t>
+  </si>
+  <si>
+    <t>Status9</t>
+  </si>
+  <si>
+    <t>Status10</t>
+  </si>
+  <si>
+    <t>Status11</t>
+  </si>
+  <si>
+    <t>Status12</t>
+  </si>
+  <si>
+    <t>Status13</t>
+  </si>
+  <si>
+    <t>Status14</t>
+  </si>
+  <si>
+    <t>Status15</t>
+  </si>
+  <si>
+    <t>Status16</t>
+  </si>
+  <si>
+    <t>Status17</t>
+  </si>
+  <si>
+    <t>Status18</t>
+  </si>
+  <si>
+    <t>Sophomore, Computer Science</t>
+  </si>
+  <si>
+    <t>Freshman, Mathematics</t>
+  </si>
+  <si>
+    <t>Junior,  Music</t>
+  </si>
+  <si>
+    <t>Sophomore, Neuroscience</t>
+  </si>
+  <si>
+    <t>Undergradte Student Instrument Project; $49,500.00</t>
+  </si>
+  <si>
+    <t>NASA Competition Project Award; $6000.00</t>
+  </si>
+  <si>
+    <t>NASA Competition Project Award; $3000.00</t>
+  </si>
+  <si>
+    <t>Undergraduate Student Instrument Project; $2750.00</t>
+  </si>
 </sst>
 </file>
 
@@ -1600,7 +1934,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1631,8 +1965,15 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1663,6 +2004,18 @@
         <bgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1683,7 +2036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1770,6 +2123,45 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2280,6 +2672,86 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="12">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="E3" s="12">
+        <v>8</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2402,7 +2874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
@@ -2593,12 +3065,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -3009,6 +3481,688 @@
         <v>1</v>
       </c>
       <c r="I14" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="3" max="3" width="38.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="87" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>347</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="85" customHeight="1">
+      <c r="A3" s="37" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>349</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" customHeight="1">
+      <c r="A4" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>352</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>353</v>
+      </c>
+      <c r="F4" s="37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="84" customHeight="1">
+      <c r="A5" s="37" t="s">
+        <v>354</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>355</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="83" customHeight="1">
+      <c r="A6" s="37" t="s">
+        <v>356</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>357</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="85" customHeight="1">
+      <c r="A7" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>358</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>359</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="85" customHeight="1">
+      <c r="A8" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>360</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="86" customHeight="1">
+      <c r="A9" s="37" t="s">
+        <v>361</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>362</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="80" customHeight="1">
+      <c r="A10" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>363</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="79" customHeight="1">
+      <c r="A11" s="37" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>366</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="80" customHeight="1">
+      <c r="A12" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>368</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>369</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="93" customHeight="1">
+      <c r="A13" s="37" t="s">
+        <v>370</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>371</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>372</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="110" customHeight="1">
+      <c r="A14" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="70" customHeight="1">
+      <c r="A15" s="37" t="s">
+        <v>373</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>374</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="73" customHeight="1">
+      <c r="A16" s="37" t="s">
+        <v>376</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>263</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>377</v>
+      </c>
+      <c r="F16" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="85" customHeight="1">
+      <c r="A17" s="37" t="s">
+        <v>378</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>379</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="91" customHeight="1">
+      <c r="A18" s="37" t="s">
+        <v>380</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>263</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>381</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="37">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AR2"/>
+  <sheetViews>
+    <sheetView topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AO3" sqref="AO3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="40" width="26.5" style="17" customWidth="1"/>
+    <col min="41" max="41" width="45.6640625" customWidth="1"/>
+    <col min="42" max="42" width="27" customWidth="1"/>
+    <col min="43" max="43" width="30.5" customWidth="1"/>
+    <col min="44" max="44" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:44">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>340</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>398</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>399</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>400</v>
+      </c>
+      <c r="N1" s="42" t="s">
+        <v>401</v>
+      </c>
+      <c r="O1" s="42" t="s">
+        <v>402</v>
+      </c>
+      <c r="P1" s="42" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q1" s="42" t="s">
+        <v>404</v>
+      </c>
+      <c r="R1" s="42" t="s">
+        <v>405</v>
+      </c>
+      <c r="S1" s="42" t="s">
+        <v>406</v>
+      </c>
+      <c r="T1" s="42" t="s">
+        <v>407</v>
+      </c>
+      <c r="U1" s="42" t="s">
+        <v>408</v>
+      </c>
+      <c r="V1" s="42" t="s">
+        <v>409</v>
+      </c>
+      <c r="W1" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y1" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z1" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA1" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB1" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC1" s="42" t="s">
+        <v>427</v>
+      </c>
+      <c r="AD1" s="42" t="s">
+        <v>428</v>
+      </c>
+      <c r="AE1" s="42" t="s">
+        <v>429</v>
+      </c>
+      <c r="AF1" s="42" t="s">
+        <v>430</v>
+      </c>
+      <c r="AG1" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="AH1" s="42" t="s">
+        <v>432</v>
+      </c>
+      <c r="AI1" s="42" t="s">
+        <v>433</v>
+      </c>
+      <c r="AJ1" s="42" t="s">
+        <v>434</v>
+      </c>
+      <c r="AK1" s="42" t="s">
+        <v>435</v>
+      </c>
+      <c r="AL1" s="42" t="s">
+        <v>436</v>
+      </c>
+      <c r="AM1" s="42" t="s">
+        <v>437</v>
+      </c>
+      <c r="AN1" s="42" t="s">
+        <v>438</v>
+      </c>
+      <c r="AO1" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP1" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ1" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="AR1" s="47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" ht="409">
+      <c r="A2" s="44" t="s">
+        <v>394</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>443</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>395</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>425</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>424</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>422</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>421</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>420</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>419</v>
+      </c>
+      <c r="M2" s="48" t="s">
+        <v>418</v>
+      </c>
+      <c r="N2" s="48" t="s">
+        <v>417</v>
+      </c>
+      <c r="O2" s="48" t="s">
+        <v>416</v>
+      </c>
+      <c r="P2" s="48" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q2" s="48" t="s">
+        <v>415</v>
+      </c>
+      <c r="R2" s="48" t="s">
+        <v>414</v>
+      </c>
+      <c r="S2" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="T2" s="48" t="s">
+        <v>412</v>
+      </c>
+      <c r="U2" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="V2" s="48" t="s">
+        <v>410</v>
+      </c>
+      <c r="W2" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="X2" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="Y2" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z2" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA2" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="AB2" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="AC2" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD2" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="AE2" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF2" s="48" t="s">
+        <v>442</v>
+      </c>
+      <c r="AG2" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH2" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="AI2" s="48" t="s">
+        <v>441</v>
+      </c>
+      <c r="AJ2" s="48" t="s">
+        <v>440</v>
+      </c>
+      <c r="AK2" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="AL2" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="AM2" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="AN2" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="AO2" s="43" t="s">
+        <v>446</v>
+      </c>
+      <c r="AP2" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AQ2" s="44">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="44" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4296,6 +5450,160 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="54.83203125" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="156" customHeight="1">
+      <c r="A2" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>444</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>382</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>384</v>
+      </c>
+      <c r="F2" s="44">
+        <v>1</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="139" customHeight="1">
+      <c r="A3" s="43" t="s">
+        <v>386</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>387</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>388</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>389</v>
+      </c>
+      <c r="F3" s="44">
+        <v>2</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="129" customHeight="1">
+      <c r="A4" s="43" t="s">
+        <v>390</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>391</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>392</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>393</v>
+      </c>
+      <c r="F4" s="44">
+        <v>4</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="135" customHeight="1">
+      <c r="A5" s="43" t="s">
+        <v>390</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>391</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>392</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>393</v>
+      </c>
+      <c r="F5" s="44">
+        <v>4</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4498,84 +5806,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" s="12">
-        <v>3</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="E3" s="12">
-        <v>8</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>